<commit_message>
Feat: Added both UIs
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="80">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,120 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bomb&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1497,9 @@
         <v>17</v>
       </c>
       <c r="G4"/>
-      <c r="H4"/>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
       <c r="I4"/>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
@@ -1601,6 +1717,278 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Feat: Added Main screen functions
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="83">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t xml:space="preserve">End&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
   </si>
 </sst>
 </file>
@@ -1748,7 +1757,7 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -1969,7 +1978,7 @@
         <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
@@ -1986,7 +1995,41 @@
         <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>